<commit_message>
Termino beam summary de corte.
</commit_message>
<xml_diff>
--- a/tests/examples/Mento-Input.xlsx
+++ b/tests/examples/Mento-Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihdi\Documents\GitHub\mento\tests\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18FA013-2FD6-4868-BF7C-4557DD54EB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A24164F-A2F4-4BD8-9D6C-8DDE49C6BF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33810" yWindow="4215" windowWidth="21555" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Beams" sheetId="1" r:id="rId1"/>
@@ -928,7 +928,7 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F14"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,7 +1106,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2">
         <v>60</v>
@@ -1159,8 +1159,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="6">
-        <f>+E7+5</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F8" s="6">
         <f>+F7+10</f>
@@ -1203,11 +1202,10 @@
         <v>40</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" ref="E9:E14" si="1">+E8+5</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" ref="F9:F14" si="2">+F8+10</f>
+        <f t="shared" ref="F9:F14" si="1">+F8+10</f>
         <v>80</v>
       </c>
       <c r="G9" s="2">
@@ -1253,11 +1251,10 @@
         <v>40</v>
       </c>
       <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
         <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="F10" s="6">
-        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="G10" s="6">
@@ -1297,11 +1294,10 @@
         <v>50</v>
       </c>
       <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G11" s="2">
@@ -1347,11 +1343,10 @@
         <v>50</v>
       </c>
       <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
         <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="F12" s="6">
-        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="G12" s="6">
@@ -1391,11 +1386,10 @@
         <v>60</v>
       </c>
       <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="F13" s="2">
-        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="G13" s="2">
@@ -1441,11 +1435,10 @@
         <v>60</v>
       </c>
       <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
         <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="F14" s="6">
-        <f t="shared" si="2"/>
         <v>130</v>
       </c>
       <c r="G14" s="6">

</xml_diff>

<commit_message>
Avance en Docs inicial
</commit_message>
<xml_diff>
--- a/tests/examples/Mento-Input.xlsx
+++ b/tests/examples/Mento-Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihdi\Documents\GitHub\mento\tests\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A24164F-A2F4-4BD8-9D6C-8DDE49C6BF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3123DBB-4E38-4DD2-974C-2EEB1FF3EE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33810" yWindow="4215" windowWidth="21555" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Beams" sheetId="1" r:id="rId1"/>
@@ -928,7 +928,7 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>